<commit_message>
Log in to Chenoa ok. GetTransaccionData ok. Procces----> DataScraping  of DateAdded and conditions ok. Several mails where configurated.
Not Done: the encompass part. Tomorrow will be working on that.

Co-Authored-By: VP-Neostella <camilo.gomez@neostella.com>
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camilo.sanchez\Documents\UiPath\PRMG_ChenoaMaxex\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cgomez\Documents\UiPath\PRMG-ChenoaInvestorStips\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA875F2B-ADC8-41D7-8D0F-C9D64B1BF4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A275E6-51A7-465E-8B8E-8017AD3F566A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="435" yWindow="2565" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -94,10 +94,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -120,9 +116,6 @@
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>vStrChenoaCredential</t>
-  </si>
-  <si>
     <t>ChenoaCredential</t>
   </si>
   <si>
@@ -132,12 +125,6 @@
     <t>PRMG</t>
   </si>
   <si>
-    <t>vStrChenoaMailRecipients</t>
-  </si>
-  <si>
-    <t>vStrChenoaMailSubject1</t>
-  </si>
-  <si>
     <t>vStrServer</t>
   </si>
   <si>
@@ -162,95 +149,77 @@
     <t>smtp-mail.outlook.com</t>
   </si>
   <si>
-    <t>vStrChenoaMailBody1</t>
-  </si>
-  <si>
-    <t>vStrChenoaMailBody2</t>
-  </si>
-  <si>
-    <t>vStrChenoaMailSubject2</t>
-  </si>
-  <si>
-    <t>vStrUrlReportsUploads</t>
-  </si>
-  <si>
-    <t>Urls</t>
-  </si>
-  <si>
-    <t>Url to go to reports and uploads.</t>
-  </si>
-  <si>
     <t>Port to read mails</t>
   </si>
   <si>
     <t>Port to send mails</t>
   </si>
   <si>
-    <t>vStrChenoaMailSubject3</t>
-  </si>
-  <si>
-    <t>vStrChenoaMailBody3</t>
-  </si>
-  <si>
-    <t>https://client.chenoafund.org/app.html?component=rowsReport&amp;type=rowsReport&amp;serverMethod=biz&amp;paneTitle=Purchase%20Conditions&amp;tabLevel1=correspondentReports&amp;tabLevel2=purchaseConditionsReport&amp;layoutVersion=purchaseConditionsReport&amp;pane=purchaseConditionsReport</t>
-  </si>
-  <si>
-    <t>vStrPathToSaveCSV</t>
-  </si>
-  <si>
     <t>Configuración</t>
   </si>
   <si>
-    <t>C:\Users\camilo.sanchez\Documents\UiPath\PRMG_ChenoaMaxex\Data\{0}.csv</t>
-  </si>
-  <si>
-    <t>vIntMaxConditions</t>
-  </si>
-  <si>
-    <t>vStrPathToSaveRemaining</t>
-  </si>
-  <si>
-    <t>vStrRemainingName</t>
-  </si>
-  <si>
-    <t>_More_than_15_conditions_for_Chenoa</t>
-  </si>
-  <si>
-    <t>vStrTotalConditionsExtract</t>
-  </si>
-  <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>SheetNameResults</t>
-  </si>
-  <si>
-    <t>Sheet1</t>
-  </si>
-  <si>
-    <t>vStrPathToSaveTotalConditions</t>
-  </si>
-  <si>
-    <t>C:\Users\camilo.sanchez\Documents\UiPath\PRMG_ChenoaMaxex\Data\{0}.xlsx</t>
-  </si>
-  <si>
-    <t>https://client.chenoafund.org/</t>
-  </si>
-  <si>
-    <t>vStrChenoaUrl</t>
-  </si>
-  <si>
     <t>ListKillApp</t>
   </si>
   <si>
     <t>Chrome</t>
+  </si>
+  <si>
+    <t>ChenoaMailRecipients</t>
+  </si>
+  <si>
+    <t>ChenoaMailBody1</t>
+  </si>
+  <si>
+    <t>ChenoaMailSubject1</t>
+  </si>
+  <si>
+    <t>ChenoaMailBody2</t>
+  </si>
+  <si>
+    <t>ChenoaMailSubject2</t>
+  </si>
+  <si>
+    <t>ChenoaMailBody3</t>
+  </si>
+  <si>
+    <t>ChenoaMailSubject3</t>
+  </si>
+  <si>
+    <t>ChenoaWebAppUrl</t>
+  </si>
+  <si>
+    <t>ChenoaUrlReportsUploads</t>
+  </si>
+  <si>
+    <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
+  </si>
+  <si>
+    <t>PathToSaveCSV</t>
+  </si>
+  <si>
+    <t>PathToSaveRemaining</t>
+  </si>
+  <si>
+    <t>MaxConditions</t>
+  </si>
+  <si>
+    <t>RemainingName</t>
+  </si>
+  <si>
+    <t>TodayDataName</t>
+  </si>
+  <si>
+    <t>_ChenoaSuspendedLoansList</t>
+  </si>
+  <si>
+    <t>_MoreThan15ConditionsForChenoa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -274,8 +243,22 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +274,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -347,17 +336,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -675,21 +665,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1002"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.6328125" customWidth="1"/>
-    <col min="3" max="3" width="102.90625" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" customWidth="1"/>
+    <col min="3" max="3" width="100.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.5">
+    <row r="1" spans="1:26" ht="18.75">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -725,16 +715,16 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.5">
+    <row r="3" spans="1:26" ht="30">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -742,188 +732,124 @@
         <v>21</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:26" s="3" customFormat="1" ht="14.25" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="3" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A6" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="15"/>
+      <c r="A6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="16"/>
       <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B7" s="8">
         <v>993</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="3" customFormat="1" ht="14.25" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B8" s="8">
         <v>587</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="15"/>
+      <c r="A10" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="16"/>
       <c r="C10" s="7"/>
     </row>
-    <row r="11" spans="1:26" ht="87">
+    <row r="11" spans="1:26" s="3" customFormat="1">
       <c r="A11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>50</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="5"/>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="7"/>
+    <row r="12" spans="1:26" s="3" customFormat="1">
+      <c r="A12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:26" ht="29">
-      <c r="A13" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="5"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="10"/>
     </row>
-    <row r="14" spans="1:26" s="3" customFormat="1" ht="29">
-      <c r="A14" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:26" s="3" customFormat="1" ht="29">
-      <c r="A15" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:26" s="3" customFormat="1" ht="14.5">
-      <c r="A16" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" s="3" customFormat="1" ht="14.5">
-      <c r="A17" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A18" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="13">
-        <v>15</v>
-      </c>
-      <c r="C18" s="13"/>
-    </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A19" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="13"/>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="13"/>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="C21" s="13"/>
-    </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="17" ht="14.25" customHeight="1"/>
+    <row r="18" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1885,20 +1811,10 @@
     <row r="991" ht="14.25" customHeight="1"/>
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
-    <row r="1002" ht="14.25" customHeight="1"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1910,14 +1826,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.453125" customWidth="1"/>
-    <col min="4" max="26" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1954,15 +1872,15 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="29">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1986,7 +1904,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -2008,7 +1926,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -2019,7 +1937,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -2030,7 +1948,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3021,28 +2939,28 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="26" width="65.453125" customWidth="1"/>
+    <col min="1" max="2" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" ht="18.75">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1"/>
@@ -3069,66 +2987,125 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" t="s">
-        <v>35</v>
-      </c>
+      <c r="A2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
+      <c r="A3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
+      <c r="A4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>46</v>
-      </c>
+      <c r="A5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="A6" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>54</v>
-      </c>
+      <c r="A7" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B9" s="12" t="s">
         <v>53</v>
       </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+    </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Start using Encompass API activities. Co-Authored-By: VP-Neostella <camilo.gomez@neostella.com>
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cgomez\Documents\UiPath\PRMG-ChenoaInvestorStips\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A275E6-51A7-465E-8B8E-8017AD3F566A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A25570-814B-4F96-9B38-CF44308E1164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="2565" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -122,24 +122,9 @@
     <t xml:space="preserve">Credentials to log in to Chenoa. </t>
   </si>
   <si>
-    <t>PRMG</t>
-  </si>
-  <si>
-    <t>vStrServer</t>
-  </si>
-  <si>
     <t>smtp.office365.com</t>
   </si>
   <si>
-    <t>Mail</t>
-  </si>
-  <si>
-    <t>vStrPortRead</t>
-  </si>
-  <si>
-    <t>vStrPortSend</t>
-  </si>
-  <si>
     <t>BotMail</t>
   </si>
   <si>
@@ -155,9 +140,6 @@
     <t>Port to send mails</t>
   </si>
   <si>
-    <t>Configuración</t>
-  </si>
-  <si>
     <t>ListKillApp</t>
   </si>
   <si>
@@ -212,7 +194,40 @@
     <t>_ChenoaSuspendedLoansList</t>
   </si>
   <si>
-    <t>_MoreThan15ConditionsForChenoa</t>
+    <t>_MoreThan15ConditionsForChenoa_</t>
+  </si>
+  <si>
+    <t>PortSend</t>
+  </si>
+  <si>
+    <t>PortRead</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>ChenoaMailSubject4</t>
+  </si>
+  <si>
+    <t>ChenoaMailBody4</t>
+  </si>
+  <si>
+    <t>MAIL</t>
+  </si>
+  <si>
+    <t>CONFIGURATION</t>
+  </si>
+  <si>
+    <t>LOGS MESSAGES</t>
+  </si>
+  <si>
+    <t>SCREEN SHOTS PATHS</t>
+  </si>
+  <si>
+    <t>ChenoaMailBody5</t>
+  </si>
+  <si>
+    <t>ChenoaMailSubject5</t>
   </si>
 </sst>
 </file>
@@ -258,7 +273,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,8 +298,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -307,16 +340,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -333,23 +376,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -668,25 +734,25 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.5703125" customWidth="1"/>
-    <col min="3" max="3" width="100.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18.75">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="22" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1"/>
@@ -713,123 +779,121 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:26" ht="30">
+      <c r="A2" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="30">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" s="2" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A5" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" s="2" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A6" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A7" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="7">
+        <v>993</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" s="2" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A8" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="7">
+        <v>587</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A9" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A10" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:26" s="2" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A11" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:26" s="2" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A12" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>55</v>
       </c>
+      <c r="C12" s="4"/>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" s="3" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A5" s="5" t="s">
+    <row r="13" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A13" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="B13" s="9" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" s="3" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A6" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="8">
-        <v>993</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" s="3" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A8" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="8">
-        <v>587</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:26" s="3" customFormat="1">
-      <c r="A11" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:26" s="3" customFormat="1">
-      <c r="A12" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="10"/>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1826,26 +1890,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" ht="22.5" customHeight="1">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="22" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1"/>
@@ -1873,81 +1937,93 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="30">
-      <c r="A2" t="s">
+      <c r="A2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
+    <row r="3" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A3" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="26"/>
+    </row>
+    <row r="4" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="25" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
+    <row r="5" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A5" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="26"/>
+    </row>
+    <row r="6" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A6" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" t="s">
+    <row r="7" spans="1:26">
+      <c r="A7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
+    <row r="8" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
+    <row r="9" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" t="s">
+    <row r="10" spans="1:26" ht="30">
+      <c r="A10" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2929,6 +3005,10 @@
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2936,10 +3016,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2950,17 +3030,17 @@
     <col min="5" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="18.75">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="10" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1"/>
@@ -2986,145 +3066,181 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A2" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A3" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A4" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A5" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A6" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A7" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A8" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B8" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="10" t="s">
+    <row r="9" spans="1:26" s="2" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A9" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:26" s="2" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A10" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:26" s="2" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A11" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:26" s="2" customFormat="1" ht="17.100000000000001" customHeight="1">
+      <c r="A12" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A13" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B13" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
     </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="10" t="s">
+    <row r="14" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A14" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B14" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="8"/>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+    <row r="15" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A15" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
+    <row r="16" spans="1:26" ht="17.100000000000001" customHeight="1">
+      <c r="A16" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A7" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
+    <row r="17" spans="1:4" ht="17.100000000000001" customHeight="1">
+      <c r="A17" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="10"/>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -4093,6 +4209,10 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
+    <row r="1003" ht="14.25" customHeight="1"/>
+    <row r="1004" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>